<commit_message>
to do map data
</commit_message>
<xml_diff>
--- a/I-SIVB-ReflectMemoryConverter/附件1-反射内存详细地址分配(the detailed address allocated to each parameter).xlsx
+++ b/I-SIVB-ReflectMemoryConverter/附件1-反射内存详细地址分配(the detailed address allocated to each parameter).xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="15" windowWidth="18135" windowHeight="11760" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="600" yWindow="15" windowWidth="18135" windowHeight="11760" tabRatio="935" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="表1-Space53" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="311">
   <si>
     <t>序号</t>
   </si>
@@ -435,9 +435,6 @@
     <t>0xF04E89-0xF04E90</t>
   </si>
   <si>
-    <t>0xF04E91-0xF04EA0</t>
-  </si>
-  <si>
     <t>0xF04EA1-0xF04EA8</t>
   </si>
   <si>
@@ -721,9 +718,6 @@
   </si>
   <si>
     <t>0x1504E89-0x1504E90</t>
-  </si>
-  <si>
-    <t>0x1504E91-0x1504EA0</t>
   </si>
   <si>
     <t>0x1504EA1-0x1504EA8</t>
@@ -1446,43 +1440,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>11 Space 52Part7</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">中数据分配
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Table 11 Address allocation of Space 52Part7</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>表</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>12 Space 52Part8</t>
     </r>
     <r>
@@ -1660,16 +1617,70 @@
     <t>This section obey CFM specification</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>表</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>11 Space 52Part7</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">中数据分配
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Table 11 Address allocation of Space 52Part7</t>
+    </r>
+  </si>
+  <si>
+    <t>ECS Bleed Configuration (TBD)</t>
+  </si>
+  <si>
+    <t>WAI Bleed Configuration (TBD)</t>
+  </si>
+  <si>
+    <t>Calibrated Air Speed (TBD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Airspeed </t>
+  </si>
+  <si>
+    <t>0x1504E91-0x1504E98</t>
+  </si>
+  <si>
+    <t>0xF04E91-0xF04E98</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1721,7 +1732,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1735,7 +1746,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1846,15 +1857,20 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1928,6 +1944,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1962,6 +1979,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2137,7 +2155,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2145,11 +2163,11 @@
       <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50.25" customHeight="1">
@@ -2159,7 +2177,7 @@
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="14.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2170,7 +2188,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2225,7 +2243,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="8" customFormat="1" ht="15">
+    <row r="8" spans="1:3" s="8" customFormat="1">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -2236,7 +2254,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15">
+    <row r="9" spans="1:3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2247,7 +2265,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15">
+    <row r="10" spans="1:3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2258,7 +2276,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15">
+    <row r="11" spans="1:3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2269,7 +2287,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2280,7 +2298,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15">
+    <row r="13" spans="1:3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2291,7 +2309,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15">
+    <row r="14" spans="1:3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2302,7 +2320,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15">
+    <row r="15" spans="1:3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2313,7 +2331,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2324,7 +2342,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2335,7 +2353,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2346,7 +2364,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2357,7 +2375,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2368,7 +2386,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2379,7 +2397,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15">
+    <row r="22" spans="1:3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2390,7 +2408,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15">
+    <row r="23" spans="1:3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2401,7 +2419,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15">
+    <row r="24" spans="1:3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -2412,7 +2430,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15">
+    <row r="25" spans="1:3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2423,7 +2441,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15">
+    <row r="26" spans="1:3" ht="30">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -2434,7 +2452,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15">
+    <row r="27" spans="1:3">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -2445,7 +2463,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -2456,7 +2474,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15">
+    <row r="29" spans="1:3">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -2467,7 +2485,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -2478,7 +2496,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
+    <row r="31" spans="1:3">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -2489,7 +2507,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15">
+    <row r="32" spans="1:3">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -2500,7 +2518,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -2511,7 +2529,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15">
+    <row r="34" spans="1:3">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2522,7 +2540,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15">
+    <row r="35" spans="1:3">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2533,7 +2551,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15">
+    <row r="36" spans="1:3">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -2544,7 +2562,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -2555,7 +2573,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15">
+    <row r="38" spans="1:3">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -2566,7 +2584,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15">
+    <row r="39" spans="1:3">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2577,7 +2595,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15">
+    <row r="40" spans="1:3">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -2588,7 +2606,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15">
+    <row r="41" spans="1:3">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -2599,7 +2617,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15">
+    <row r="42" spans="1:3">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -2610,7 +2628,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15">
+    <row r="43" spans="1:3">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -2621,7 +2639,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15">
+    <row r="44" spans="1:3">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -2632,7 +2650,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15">
+    <row r="45" spans="1:3">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -2643,7 +2661,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15">
+    <row r="46" spans="1:3">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -2654,7 +2672,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15">
+    <row r="47" spans="1:3">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -2665,7 +2683,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15">
+    <row r="48" spans="1:3">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -4325,7 +4343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4334,23 +4352,23 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>46</v>
@@ -4359,15 +4377,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -4375,10 +4393,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1">
@@ -4386,10 +4404,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1">
@@ -4397,10 +4415,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1">
@@ -6265,32 +6283,32 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N30" sqref="N30"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>46</v>
@@ -6299,15 +6317,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -6315,10 +6333,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>271</v>
+        <v>305</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1">
@@ -6326,10 +6344,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>272</v>
+        <v>306</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1">
@@ -6337,10 +6355,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1">
@@ -8205,7 +8223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8214,23 +8232,23 @@
       <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>46</v>
@@ -8239,15 +8257,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -8255,10 +8273,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1">
@@ -8266,10 +8284,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1">
@@ -8277,10 +8295,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1">
@@ -10145,32 +10163,32 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N30" sqref="N30"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>46</v>
@@ -10184,10 +10202,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -10195,7 +10213,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -10204,7 +10222,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -10213,7 +10231,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -12079,7 +12097,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12088,23 +12106,23 @@
       <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>46</v>
@@ -12118,10 +12136,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -12129,7 +12147,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -12138,7 +12156,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -12147,7 +12165,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -14013,7 +14031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14022,23 +14040,23 @@
       <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>46</v>
@@ -14052,10 +14070,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -14063,7 +14081,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -14072,7 +14090,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -14081,7 +14099,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -15947,29 +15965,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D593"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="14.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -15980,7 +15998,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -16035,7 +16053,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="8" customFormat="1" ht="15">
+    <row r="8" spans="1:3" s="8" customFormat="1">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -16046,7 +16064,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15">
+    <row r="9" spans="1:3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -16054,10 +16072,10 @@
         <v>49</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -16065,10 +16083,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -16076,10 +16094,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -16087,10 +16105,10 @@
         <v>43</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -16098,10 +16116,10 @@
         <v>44</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -16109,10 +16127,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -16120,10 +16138,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -16131,10 +16149,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -16142,10 +16160,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -16153,10 +16171,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -16164,10 +16182,10 @@
         <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -16175,10 +16193,10 @@
         <v>13</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -16186,10 +16204,10 @@
         <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -16197,10 +16215,10 @@
         <v>15</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -16208,10 +16226,10 @@
         <v>16</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -16219,10 +16237,10 @@
         <v>17</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -16230,10 +16248,10 @@
         <v>18</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -16241,10 +16259,10 @@
         <v>19</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -16252,10 +16270,10 @@
         <v>20</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -16263,10 +16281,10 @@
         <v>21</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -16274,10 +16292,10 @@
         <v>22</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -16285,10 +16303,10 @@
         <v>23</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -16296,10 +16314,10 @@
         <v>24</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -16307,10 +16325,10 @@
         <v>25</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -16318,10 +16336,10 @@
         <v>26</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -16329,10 +16347,10 @@
         <v>27</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -16340,10 +16358,10 @@
         <v>28</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -16351,10 +16369,10 @@
         <v>29</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -16362,10 +16380,10 @@
         <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -16373,10 +16391,10 @@
         <v>31</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -16384,10 +16402,10 @@
         <v>32</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -16395,10 +16413,10 @@
         <v>33</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -16406,10 +16424,10 @@
         <v>34</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -16417,10 +16435,10 @@
         <v>35</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -16428,10 +16446,10 @@
         <v>36</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -16439,10 +16457,10 @@
         <v>37</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -16450,10 +16468,10 @@
         <v>38</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -16461,10 +16479,10 @@
         <v>39</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -16472,10 +16490,10 @@
         <v>40</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -16483,7 +16501,7 @@
         <v>41</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="3:4">
@@ -18135,29 +18153,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="14.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -18168,7 +18186,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -18176,7 +18194,7 @@
         <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1">
@@ -18187,7 +18205,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.5" customHeight="1">
@@ -18198,7 +18216,7 @@
         <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="20.25" customHeight="1">
@@ -18209,7 +18227,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21" customHeight="1">
@@ -18220,10 +18238,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="8" customFormat="1" ht="15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="8" customFormat="1">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -18231,10 +18249,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -18242,10 +18260,10 @@
         <v>49</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -18253,10 +18271,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -18264,10 +18282,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -18275,10 +18293,10 @@
         <v>43</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -18286,10 +18304,10 @@
         <v>44</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -18297,10 +18315,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -18308,10 +18326,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -18319,10 +18337,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -18330,10 +18348,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -18341,10 +18359,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -18352,10 +18370,10 @@
         <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -18363,10 +18381,10 @@
         <v>13</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -18374,10 +18392,10 @@
         <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -18385,10 +18403,10 @@
         <v>15</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -18396,10 +18414,10 @@
         <v>16</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -18407,10 +18425,10 @@
         <v>17</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -18418,10 +18436,10 @@
         <v>18</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -18429,10 +18447,10 @@
         <v>19</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -18440,10 +18458,10 @@
         <v>20</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -18451,10 +18469,10 @@
         <v>21</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -18462,10 +18480,10 @@
         <v>22</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -18473,10 +18491,10 @@
         <v>23</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -18484,10 +18502,10 @@
         <v>24</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -18495,10 +18513,10 @@
         <v>25</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -18506,10 +18524,10 @@
         <v>26</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -18517,10 +18535,10 @@
         <v>27</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -18528,10 +18546,10 @@
         <v>28</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -18539,10 +18557,10 @@
         <v>29</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -18550,10 +18568,10 @@
         <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -18561,10 +18579,10 @@
         <v>31</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -18572,10 +18590,10 @@
         <v>32</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -18583,10 +18601,10 @@
         <v>33</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -18594,10 +18612,10 @@
         <v>34</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -18605,10 +18623,10 @@
         <v>35</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -18616,10 +18634,10 @@
         <v>36</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -18627,10 +18645,10 @@
         <v>37</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -18638,10 +18656,10 @@
         <v>38</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -18649,10 +18667,10 @@
         <v>39</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -18660,10 +18678,10 @@
         <v>40</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -18671,7 +18689,7 @@
         <v>41</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="3:4">
@@ -20323,29 +20341,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="14.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -20356,7 +20374,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -20364,7 +20382,7 @@
         <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1">
@@ -20375,7 +20393,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.5" customHeight="1">
@@ -20386,7 +20404,7 @@
         <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="20.25" customHeight="1">
@@ -20397,7 +20415,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21" customHeight="1">
@@ -20408,10 +20426,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="8" customFormat="1" ht="15">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="8" customFormat="1">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -20419,21 +20437,21 @@
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>49</v>
+        <v>308</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -20441,10 +20459,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -20452,10 +20470,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -20463,10 +20481,10 @@
         <v>43</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -20474,10 +20492,10 @@
         <v>44</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -20485,10 +20503,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -20496,10 +20514,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -20507,10 +20525,10 @@
         <v>9</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -20518,10 +20536,10 @@
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -20529,10 +20547,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -20540,10 +20558,10 @@
         <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -20551,10 +20569,10 @@
         <v>13</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -20562,10 +20580,10 @@
         <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -20573,10 +20591,10 @@
         <v>15</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -20584,10 +20602,10 @@
         <v>16</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -20595,10 +20613,10 @@
         <v>17</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -20606,10 +20624,10 @@
         <v>18</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -20617,10 +20635,10 @@
         <v>19</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -20628,10 +20646,10 @@
         <v>20</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -20639,10 +20657,10 @@
         <v>21</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -20650,10 +20668,10 @@
         <v>22</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -20661,10 +20679,10 @@
         <v>23</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -20672,10 +20690,10 @@
         <v>24</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -20683,10 +20701,10 @@
         <v>25</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -20694,10 +20712,10 @@
         <v>26</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -20705,10 +20723,10 @@
         <v>27</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -20716,10 +20734,10 @@
         <v>28</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -20727,10 +20745,10 @@
         <v>29</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -20738,10 +20756,10 @@
         <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -20749,10 +20767,10 @@
         <v>31</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -20760,10 +20778,10 @@
         <v>32</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -20771,10 +20789,10 @@
         <v>33</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -20782,10 +20800,10 @@
         <v>34</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -20793,10 +20811,10 @@
         <v>35</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -20804,10 +20822,10 @@
         <v>36</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -20815,10 +20833,10 @@
         <v>37</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -20826,10 +20844,10 @@
         <v>38</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -20837,10 +20855,10 @@
         <v>39</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -20848,10 +20866,10 @@
         <v>40</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -20859,7 +20877,7 @@
         <v>41</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="3:4">
@@ -22511,7 +22529,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22519,21 +22537,21 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -22544,15 +22562,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -22560,10 +22578,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1">
@@ -22571,10 +22589,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1">
@@ -22582,10 +22600,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1">
@@ -24450,7 +24468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24458,21 +24476,21 @@
       <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -24483,15 +24501,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -24499,10 +24517,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1">
@@ -24510,10 +24528,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1">
@@ -24521,10 +24539,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1">
@@ -24532,35 +24550,35 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" ht="15">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -26407,7 +26425,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26415,21 +26433,21 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -26440,15 +26458,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -26456,10 +26474,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1">
@@ -26467,10 +26485,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1">
@@ -26478,10 +26496,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1">
@@ -26489,35 +26507,35 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" ht="15">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -28364,7 +28382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28372,21 +28390,21 @@
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -28397,15 +28415,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -28413,10 +28431,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1">
@@ -28424,10 +28442,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1">
@@ -28435,10 +28453,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1">
@@ -28446,35 +28464,35 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" ht="15">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -30321,7 +30339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F593"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -30329,21 +30347,21 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="51.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -30354,15 +30372,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
@@ -30370,10 +30388,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1">
@@ -30381,10 +30399,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1">
@@ -30392,10 +30410,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1">
@@ -30403,35 +30421,35 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" ht="15">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:6">

</xml_diff>